<commit_message>
Scheduler now prefers to schedule games at earlier times than later times. Also changed the config.ini file and bigBook2013.xlsx to strings for conferences instead of ints. Also put in team codes instead of team names in the "Not Same Time As" column so the scheduler now doesn't schedule those teams at the same time (both in smallBook.xlsx and bigBook2013.xlsx).
</commit_message>
<xml_diff>
--- a/smallBook.xlsx
+++ b/smallBook.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="90">
   <si>
     <t>TEAM  LIST  AS  OF :</t>
   </si>
@@ -181,9 +180,6 @@
     <t>No 1/7/13-1/8/13, no 1/14/13-1/15/13, no 1/27/13-1/29/13, no 2/10/13-2/12/13, no 2/25/13-2/27/13</t>
   </si>
   <si>
-    <t>BOOMER BOMBERS</t>
-  </si>
-  <si>
     <t>2015-GOLDEN BEARS</t>
   </si>
   <si>
@@ -226,9 +222,6 @@
     <t>205-OUTLAWS 2B</t>
   </si>
   <si>
-    <t>Outlaws 2A if possible</t>
-  </si>
-  <si>
     <t>2011-LIBERATORS-GABANI 2</t>
   </si>
   <si>
@@ -271,9 +264,6 @@
     <t>NO 1/7/13-1/8/13, NO 1/12/13, NO 1/14/13-1/15/13, NO 1/27/13-1/29/13, NO 2/10/13-2/12/13, no 2/25/13-2/27/13</t>
   </si>
   <si>
-    <t>WILDCATS-SCOTT 2</t>
-  </si>
-  <si>
     <t>223-EAGLES-TURNER 2</t>
   </si>
   <si>
@@ -290,9 +280,6 @@
   </si>
   <si>
     <t>225-OUTLAWS 2A</t>
-  </si>
-  <si>
-    <t>Outlaws 2B if possible</t>
   </si>
   <si>
     <t>226-TIGER PRIDE 2</t>
@@ -304,15 +291,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="\$#,##0.00" numFmtId="166"/>
-    <numFmt formatCode="D\-MMM;@" numFmtId="167"/>
-    <numFmt formatCode="D\-MMM" numFmtId="168"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -321,53 +305,38 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Berlin Sans FB"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Berlin Sans FB"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="9"/>
       <name val="Berlin Sans FB"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -387,7 +356,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Wingdings 2"/>
       <family val="1"/>
@@ -413,7 +382,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Wingdings 2"/>
       <family val="1"/>
@@ -427,7 +396,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="9"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -443,337 +412,216 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="165">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="166" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="12" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="13" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="13" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="13">
     <dxf>
       <font>
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -785,175 +633,8 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -965,10 +646,125 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C6500"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C6500"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -980,10 +776,8 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
-      <numFmt formatCode="GENERAL" numFmtId="165"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -991,6 +785,7 @@
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1049,39 +844,334 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H30" activeCellId="0" pane="topLeft" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.54081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.18367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.81122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="124.540816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.8163265306122"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.4540816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.72959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="13.140625"/>
+    <col min="3" max="3" width="31.28515625"/>
+    <col min="4" max="4" width="8.7109375"/>
+    <col min="5" max="5" width="7.5703125"/>
+    <col min="6" max="6" width="7.140625"/>
+    <col min="7" max="7" width="5.85546875"/>
+    <col min="8" max="8" width="124.5703125"/>
+    <col min="9" max="9" width="20.85546875"/>
+    <col min="10" max="11" width="11.42578125"/>
+    <col min="12" max="12" width="9.7109375"/>
+    <col min="13" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="1">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1182,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16" outlineLevel="0" r="2">
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -1130,8 +1220,8 @@
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
-      <c r="A3" s="17" t="n">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
         <v>101</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -1144,7 +1234,7 @@
       <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="18" t="n">
+      <c r="F3" s="18">
         <v>1</v>
       </c>
       <c r="G3" s="18" t="s">
@@ -1164,8 +1254,8 @@
       <c r="S3" s="30"/>
       <c r="T3" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
-      <c r="A4" s="17" t="n">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
         <v>102</v>
       </c>
       <c r="B4" s="18" t="s">
@@ -1178,7 +1268,7 @@
       <c r="E4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="18" t="n">
+      <c r="F4" s="18">
         <v>1</v>
       </c>
       <c r="G4" s="18" t="s">
@@ -1200,8 +1290,8 @@
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
-      <c r="A5" s="17" t="n">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>103</v>
       </c>
       <c r="B5" s="18" t="s">
@@ -1214,7 +1304,7 @@
       <c r="E5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="18" t="n">
+      <c r="F5" s="18">
         <v>1</v>
       </c>
       <c r="G5" s="18" t="s">
@@ -1236,8 +1326,8 @@
       <c r="S5" s="30"/>
       <c r="T5" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="6">
-      <c r="A6" s="17" t="n">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>104</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -1250,7 +1340,7 @@
       <c r="E6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="18" t="n">
+      <c r="F6" s="18">
         <v>1</v>
       </c>
       <c r="G6" s="18" t="s">
@@ -1272,8 +1362,8 @@
       <c r="S6" s="30"/>
       <c r="T6" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="7">
-      <c r="A7" s="17" t="n">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>105</v>
       </c>
       <c r="B7" s="18" t="s">
@@ -1286,7 +1376,7 @@
       <c r="E7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="18" t="n">
+      <c r="F7" s="18">
         <v>1</v>
       </c>
       <c r="G7" s="18" t="s">
@@ -1310,8 +1400,8 @@
       <c r="S7" s="30"/>
       <c r="T7" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
-      <c r="A8" s="17" t="n">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>106</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -1324,7 +1414,7 @@
       <c r="E8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="18" t="n">
+      <c r="F8" s="18">
         <v>1</v>
       </c>
       <c r="G8" s="18" t="s">
@@ -1346,8 +1436,8 @@
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
-      <c r="A9" s="17" t="n">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
         <v>107</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -1360,7 +1450,7 @@
       <c r="E9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="18" t="n">
+      <c r="F9" s="18">
         <v>1</v>
       </c>
       <c r="G9" s="18" t="s">
@@ -1382,8 +1472,8 @@
       <c r="S9" s="30"/>
       <c r="T9" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
-      <c r="A10" s="17" t="n">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
         <v>141</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -1396,7 +1486,7 @@
       <c r="E10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="18" t="n">
+      <c r="F10" s="18">
         <v>1</v>
       </c>
       <c r="G10" s="18" t="s">
@@ -1416,8 +1506,8 @@
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
-      <c r="A11" s="17" t="n">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>142</v>
       </c>
       <c r="B11" s="44" t="s">
@@ -1430,7 +1520,7 @@
       <c r="E11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="18" t="n">
+      <c r="F11" s="18">
         <v>1</v>
       </c>
       <c r="G11" s="18" t="s">
@@ -1454,8 +1544,8 @@
       <c r="S11" s="30"/>
       <c r="T11" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
-      <c r="A12" s="17" t="n">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>143</v>
       </c>
       <c r="B12" s="44" t="s">
@@ -1468,7 +1558,7 @@
       <c r="E12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="18" t="n">
+      <c r="F12" s="18">
         <v>1</v>
       </c>
       <c r="G12" s="18" t="s">
@@ -1490,8 +1580,8 @@
       <c r="S12" s="30"/>
       <c r="T12" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
-      <c r="A13" s="17" t="n">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>145</v>
       </c>
       <c r="B13" s="44" t="s">
@@ -1504,7 +1594,7 @@
       <c r="E13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="18" t="n">
+      <c r="F13" s="18">
         <v>1</v>
       </c>
       <c r="G13" s="18" t="s">
@@ -1526,8 +1616,8 @@
       <c r="S13" s="30"/>
       <c r="T13" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="14">
-      <c r="A14" s="17" t="n">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <v>146</v>
       </c>
       <c r="B14" s="44" t="s">
@@ -1540,7 +1630,7 @@
       <c r="E14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="18" t="n">
+      <c r="F14" s="18">
         <v>1</v>
       </c>
       <c r="G14" s="18" t="s">
@@ -1562,8 +1652,8 @@
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="15">
-      <c r="A15" s="17" t="n">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
         <v>151</v>
       </c>
       <c r="B15" s="44" t="s">
@@ -1576,7 +1666,7 @@
       <c r="E15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="18" t="n">
+      <c r="F15" s="18">
         <v>1</v>
       </c>
       <c r="G15" s="18" t="s">
@@ -1598,8 +1688,8 @@
       <c r="S15" s="30"/>
       <c r="T15" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
-      <c r="A16" s="17" t="n">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
         <v>152</v>
       </c>
       <c r="B16" s="44" t="s">
@@ -1612,7 +1702,7 @@
       <c r="E16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="18" t="n">
+      <c r="F16" s="18">
         <v>1</v>
       </c>
       <c r="G16" s="18" t="s">
@@ -1632,8 +1722,8 @@
       <c r="S16" s="30"/>
       <c r="T16" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
-      <c r="A17" s="17" t="n">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
         <v>153</v>
       </c>
       <c r="B17" s="44" t="s">
@@ -1646,7 +1736,7 @@
       <c r="E17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="18" t="n">
+      <c r="F17" s="18">
         <v>1</v>
       </c>
       <c r="G17" s="18" t="s">
@@ -1666,8 +1756,8 @@
       <c r="S17" s="30"/>
       <c r="T17" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="18">
-      <c r="A18" s="17" t="n">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
         <v>154</v>
       </c>
       <c r="B18" s="44" t="s">
@@ -1680,7 +1770,7 @@
       <c r="E18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="18" t="n">
+      <c r="F18" s="18">
         <v>1</v>
       </c>
       <c r="G18" s="18" t="s">
@@ -1700,8 +1790,8 @@
       <c r="S18" s="30"/>
       <c r="T18" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="19">
-      <c r="A19" s="17" t="n">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
         <v>155</v>
       </c>
       <c r="B19" s="44" t="s">
@@ -1714,7 +1804,7 @@
       <c r="E19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="18" t="n">
+      <c r="F19" s="18">
         <v>1</v>
       </c>
       <c r="G19" s="18" t="s">
@@ -1734,8 +1824,8 @@
       <c r="S19" s="30"/>
       <c r="T19" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="20">
-      <c r="A20" s="17" t="n">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
         <v>156</v>
       </c>
       <c r="B20" s="44" t="s">
@@ -1748,7 +1838,7 @@
       <c r="E20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="18" t="n">
+      <c r="F20" s="18">
         <v>1</v>
       </c>
       <c r="G20" s="18" t="s">
@@ -1768,8 +1858,8 @@
       <c r="S20" s="30"/>
       <c r="T20" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="21">
-      <c r="A21" s="17" t="n">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
         <v>208</v>
       </c>
       <c r="B21" s="44" t="s">
@@ -1782,7 +1872,7 @@
       <c r="E21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="18" t="n">
+      <c r="F21" s="18">
         <v>2</v>
       </c>
       <c r="G21" s="18" t="s">
@@ -1804,8 +1894,8 @@
       <c r="S21" s="30"/>
       <c r="T21" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="22">
-      <c r="A22" s="17" t="n">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
         <v>207</v>
       </c>
       <c r="B22" s="44" t="s">
@@ -1818,7 +1908,7 @@
       <c r="E22" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="18">
         <v>2</v>
       </c>
       <c r="G22" s="18" t="s">
@@ -1838,8 +1928,8 @@
       <c r="S22" s="30"/>
       <c r="T22" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="23">
-      <c r="A23" s="17" t="n">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
         <v>2014</v>
       </c>
       <c r="B23" s="44" t="s">
@@ -1852,7 +1942,7 @@
       <c r="E23" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="18" t="n">
+      <c r="F23" s="18">
         <v>2</v>
       </c>
       <c r="G23" s="18" t="s">
@@ -1861,8 +1951,8 @@
       <c r="H23" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I23" s="43" t="s">
-        <v>54</v>
+      <c r="I23" s="43">
+        <v>222</v>
       </c>
       <c r="J23" s="42"/>
       <c r="K23" s="23"/>
@@ -1876,21 +1966,21 @@
       <c r="S23" s="30"/>
       <c r="T23" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="24">
-      <c r="A24" s="17" t="n">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
         <v>2015</v>
       </c>
       <c r="B24" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="18" t="n">
+      <c r="F24" s="18">
         <v>2</v>
       </c>
       <c r="G24" s="18" t="s">
@@ -1910,21 +2000,21 @@
       <c r="S24" s="30"/>
       <c r="T24" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="25">
-      <c r="A25" s="17" t="n">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
         <v>2016</v>
       </c>
       <c r="B25" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="18" t="n">
+      <c r="F25" s="18">
         <v>2</v>
       </c>
       <c r="G25" s="18" t="s">
@@ -1944,28 +2034,28 @@
       <c r="S25" s="30"/>
       <c r="T25" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="26">
-      <c r="A26" s="17" t="n">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
         <v>2013</v>
       </c>
       <c r="B26" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="18" t="n">
+      <c r="F26" s="18">
         <v>2</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="22"/>
@@ -1980,21 +2070,21 @@
       <c r="S26" s="30"/>
       <c r="T26" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="27">
-      <c r="A27" s="17" t="n">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
         <v>203</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="18" t="n">
+      <c r="F27" s="18">
         <v>2</v>
       </c>
       <c r="G27" s="18" t="s">
@@ -2014,28 +2104,28 @@
       <c r="S27" s="30"/>
       <c r="T27" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="28">
-      <c r="A28" s="48" t="n">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="48">
         <v>2012</v>
       </c>
       <c r="B28" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="18" t="n">
+      <c r="F28" s="18">
         <v>2</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="49"/>
@@ -2050,28 +2140,28 @@
       <c r="S28" s="30"/>
       <c r="T28" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="29">
-      <c r="A29" s="55" t="n">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="55">
         <v>206</v>
       </c>
       <c r="B29" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="43" t="s">
         <v>62</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>63</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="18" t="n">
+      <c r="F29" s="18">
         <v>2</v>
       </c>
       <c r="G29" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H29" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I29" s="43"/>
       <c r="J29" s="42"/>
@@ -2086,28 +2176,28 @@
       <c r="S29" s="30"/>
       <c r="T29" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="30">
-      <c r="A30" s="17" t="n">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
         <v>202</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="18" t="n">
+      <c r="F30" s="18">
         <v>2</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="22"/>
@@ -2122,28 +2212,28 @@
       <c r="S30" s="30"/>
       <c r="T30" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.5" outlineLevel="0" r="31">
-      <c r="A31" s="17" t="n">
+    <row r="31" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
         <v>2010</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="18" t="n">
+      <c r="F31" s="18">
         <v>2</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="49"/>
@@ -2158,29 +2248,29 @@
       <c r="S31" s="30"/>
       <c r="T31" s="57"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="32">
-      <c r="A32" s="17" t="n">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
         <v>205</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="18" t="n">
+      <c r="F32" s="18">
         <v>2</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H32" s="21"/>
-      <c r="I32" s="3" t="s">
-        <v>69</v>
+      <c r="I32" s="3">
+        <v>225</v>
       </c>
       <c r="J32" s="49"/>
       <c r="K32" s="23"/>
@@ -2194,28 +2284,28 @@
       <c r="S32" s="30"/>
       <c r="T32" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="33">
-      <c r="A33" s="17" t="n">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
         <v>2011</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="18" t="n">
+      <c r="F33" s="18">
         <v>2</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I33" s="43"/>
       <c r="J33" s="42"/>
@@ -2230,28 +2320,28 @@
       <c r="S33" s="30"/>
       <c r="T33" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="34">
-      <c r="A34" s="17" t="n">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
         <v>209</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="18" t="n">
+      <c r="F34" s="18">
         <v>2</v>
       </c>
       <c r="G34" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I34" s="43"/>
       <c r="J34" s="42"/>
@@ -2266,21 +2356,21 @@
       <c r="S34" s="30"/>
       <c r="T34" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="35">
-      <c r="A35" s="17" t="n">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
         <v>204</v>
       </c>
       <c r="B35" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="18" t="n">
+      <c r="F35" s="18">
         <v>2</v>
       </c>
       <c r="G35" s="18" t="s">
@@ -2300,31 +2390,31 @@
       <c r="S35" s="30"/>
       <c r="T35" s="64"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="36">
-      <c r="A36" s="17" t="n">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
         <v>201</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="18">
         <v>2</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J36" s="33"/>
       <c r="K36" s="23"/>
@@ -2338,31 +2428,31 @@
       <c r="S36" s="30"/>
       <c r="T36" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="37">
-      <c r="A37" s="17" t="n">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
         <v>221</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="65" t="n">
+      <c r="F37" s="65">
         <v>2</v>
       </c>
       <c r="G37" s="65" t="s">
         <v>19</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I37" s="43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J37" s="42"/>
       <c r="K37" s="23"/>
@@ -2376,31 +2466,31 @@
       <c r="S37" s="30"/>
       <c r="T37" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="38">
-      <c r="A38" s="17" t="n">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
         <v>222</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="18" t="n">
+      <c r="F38" s="18">
         <v>2</v>
       </c>
       <c r="G38" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" s="43" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="I38" s="43">
+        <v>2014</v>
       </c>
       <c r="J38" s="42"/>
       <c r="K38" s="23"/>
@@ -2414,21 +2504,21 @@
       <c r="S38" s="30"/>
       <c r="T38" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="39">
-      <c r="A39" s="17" t="n">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
         <v>223</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="18" t="n">
+      <c r="F39" s="18">
         <v>2</v>
       </c>
       <c r="G39" s="18" t="s">
@@ -2436,7 +2526,7 @@
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J39" s="33"/>
       <c r="K39" s="23"/>
@@ -2450,31 +2540,31 @@
       <c r="S39" s="30"/>
       <c r="T39" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="40">
-      <c r="A40" s="17" t="n">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
         <v>224</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="18" t="n">
+      <c r="F40" s="18">
         <v>2</v>
       </c>
       <c r="G40" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I40" s="43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J40" s="33"/>
       <c r="K40" s="23"/>
@@ -2488,29 +2578,29 @@
       <c r="S40" s="30"/>
       <c r="T40" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="41">
-      <c r="A41" s="17" t="n">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
         <v>225</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="18" t="n">
+      <c r="F41" s="18">
         <v>2</v>
       </c>
       <c r="G41" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H41" s="21"/>
-      <c r="I41" s="3" t="s">
-        <v>91</v>
+      <c r="I41" s="3">
+        <v>205</v>
       </c>
       <c r="J41" s="49"/>
       <c r="K41" s="23"/>
@@ -2524,28 +2614,28 @@
       <c r="S41" s="30"/>
       <c r="T41" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="42">
-      <c r="A42" s="55" t="n">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="55">
         <v>226</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="18" t="n">
+      <c r="F42" s="18">
         <v>2</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I42" s="43"/>
       <c r="J42" s="42"/>
@@ -2562,130 +2652,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" operator="duplicateValues" percent="0" priority="2" rank="0" text="" type="duplicateValues">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule aboveAverage="0" bottom="0" dxfId="1" equalAverage="0" operator="duplicateValues" percent="0" priority="3" rank="0" text="" type="duplicateValues">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2,R4:R9">
-    <cfRule aboveAverage="0" bottom="0" dxfId="2" equalAverage="0" operator="equal" percent="0" priority="4" rank="0" text="" type="cellIs">
+  <conditionalFormatting sqref="R2:R9">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R9">
-    <cfRule aboveAverage="0" bottom="0" dxfId="3" equalAverage="0" operator="equal" percent="0" priority="5" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R9">
-    <cfRule aboveAverage="0" bottom="0" dxfId="4" equalAverage="0" operator="lessThan" percent="0" priority="6" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="5" equalAverage="0" operator="greaterThan" percent="0" priority="7" rank="0" text="" type="cellIs">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="6" equalAverage="0" operator="lessThan" percent="0" priority="8" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R42">
-    <cfRule aboveAverage="0" bottom="0" dxfId="7" equalAverage="0" operator="equal" percent="0" priority="9" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R42">
-    <cfRule aboveAverage="0" bottom="0" dxfId="8" equalAverage="0" operator="equal" percent="0" priority="10" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R42">
-    <cfRule aboveAverage="0" bottom="0" dxfId="9" equalAverage="0" operator="lessThan" percent="0" priority="11" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="10" equalAverage="0" operator="greaterThan" percent="0" priority="12" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="11" equalAverage="0" operator="lessThan" percent="0" priority="13" rank="0" text="" type="cellIs">
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule aboveAverage="0" bottom="0" dxfId="12" equalAverage="0" operator="duplicateValues" percent="0" priority="14" rank="0" text="" type="duplicateValues">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H39,H10,H25:H27">
-    <cfRule aboveAverage="0" bottom="0" dxfId="13" equalAverage="0" operator="duplicateValues" percent="0" priority="15" rank="0" text="" type="duplicateValues">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="1" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule aboveAverage="0" bottom="0" dxfId="14" equalAverage="0" operator="duplicateValues" percent="0" priority="16" rank="0" text="" type="duplicateValues">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed DH/B2B to a hard constraint.
</commit_message>
<xml_diff>
--- a/smallBook.xlsx
+++ b/smallBook.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="86">
   <si>
     <t>TEAM  LIST  AS  OF :</t>
   </si>
@@ -57,6 +58,9 @@
     <t>R</t>
   </si>
   <si>
+    <t>B2B</t>
+  </si>
+  <si>
     <t>102-BULLS-SHORTER</t>
   </si>
   <si>
@@ -78,16 +82,16 @@
     <t>I</t>
   </si>
   <si>
-    <t>no 1/10/13-1/13/13, no 1/6/13</t>
+    <t>No 11/10/13-11/13/13, no 11/6/13</t>
   </si>
   <si>
     <t>105-IRISH-WEBSTER 1</t>
   </si>
   <si>
-    <t>No 1/12/13, only before 10:00pm</t>
-  </si>
-  <si>
-    <t>Irish 2, Bears 3</t>
+    <t>No 11/12/13, only before 10:00pm</t>
+  </si>
+  <si>
+    <t>103, 207</t>
   </si>
   <si>
     <t>106-PATRIOTS</t>
@@ -111,16 +115,13 @@
     <t>142-MISSOURI WINGS 1</t>
   </si>
   <si>
-    <t>no 1/4/13, no 2/4/13, no 2/18/13</t>
-  </si>
-  <si>
-    <t>WINGS 2</t>
+    <t>no 11/4/13, no 12/4/13, no 12/18/13</t>
   </si>
   <si>
     <t>143-PANTHERS</t>
   </si>
   <si>
-    <t>NO 1/14/13-1/15/13, NO 1/21/13-1/22/13, NO 2/11/13-2/12/13, NO 2/24/13-2/25/13</t>
+    <t>NO 11/14/13-11/15/13, NO 11/21/13-11/22/13, NO 12/11/13-12/12/13, NO 12/24/13-12/25/13</t>
   </si>
   <si>
     <t>145-THUNDER-CAMPBELL</t>
@@ -132,7 +133,7 @@
     <t>146-THUNDER-CRIGHTON</t>
   </si>
   <si>
-    <t>No 1/21/13-1/22/13, NO Saturday</t>
+    <t>No 11/21/13-11/22/13, NO Saturday</t>
   </si>
   <si>
     <t>1c</t>
@@ -144,7 +145,7 @@
     <t>G</t>
   </si>
   <si>
-    <t>No 2/16/13-2/18/13</t>
+    <t>No 12/16/13-12/18/13</t>
   </si>
   <si>
     <t>152-LITTLE PURPLE THUNDER</t>
@@ -168,7 +169,7 @@
     <t>208-YELLOWJACKETS-WILSON</t>
   </si>
   <si>
-    <t>NO 2/17/13-2/25/13, DH</t>
+    <t>NO 12/17/13-12/25/13, DH</t>
   </si>
   <si>
     <t>207-THE BEARS-BURRI</t>
@@ -177,7 +178,7 @@
     <t>2014-WILDCATS-SCOTT 2</t>
   </si>
   <si>
-    <t>No 1/7/13-1/8/13, no 1/14/13-1/15/13, no 1/27/13-1/29/13, no 2/10/13-2/12/13, no 2/25/13-2/27/13</t>
+    <t>No 11/7/13-11/8/13, no 11/14/13-11/15/13, no 11/27/13-11/29/13, no 12/10/13-12/12/13, no 12/25/13-12/27/13</t>
   </si>
   <si>
     <t>2015-GOLDEN BEARS</t>
@@ -210,13 +211,10 @@
     <t>202-CRUSH-TREAT 2</t>
   </si>
   <si>
-    <t>VERY new team and inexperienced team :)</t>
-  </si>
-  <si>
     <t>2010-EAGLES-PIPER 2</t>
   </si>
   <si>
-    <t>DH, NO 2/16/13, NO 2/23/13</t>
+    <t>DH, NO 12/16/13, NO 12/23/13</t>
   </si>
   <si>
     <t>205-OUTLAWS 2B</t>
@@ -225,13 +223,13 @@
     <t>2011-LIBERATORS-GABANI 2</t>
   </si>
   <si>
-    <t>DH, no 2/19/13</t>
+    <t>DH, no 12/19/13</t>
   </si>
   <si>
     <t>209-GENERALS-BOSWELL</t>
   </si>
   <si>
-    <t>NO 2/18/13</t>
+    <t>NO 12/18/13</t>
   </si>
   <si>
     <t>204-LAKERS-SWEATT</t>
@@ -240,10 +238,7 @@
     <t>201-BLUEJAYS-HUTTER</t>
   </si>
   <si>
-    <t>no 1/1/13-1/15/13, NO 2/16/13-2/25/13, No Saturday,  No 4:40, pref after 5:30pm</t>
-  </si>
-  <si>
-    <t>BLUJAYS DUNCAN-REID</t>
+    <t>no 11/1/13-11/15/13, NO 12/16/13-12/25/13, No Saturday,  No 4:40, pref after 5:30pm</t>
   </si>
   <si>
     <t>2c</t>
@@ -252,28 +247,22 @@
     <t>221-BLUEJAYS-DUNCAN-REID</t>
   </si>
   <si>
-    <t>No 1/1/13-1/15/13, NO 2/16/13-2/25/13, No 4:40, only before 5:30pm</t>
-  </si>
-  <si>
-    <t>BLUEJAYS-HUTTER OR BAILEY</t>
+    <t>No 11/1/13-11/15/13, NO 12/16/13-12/25/13, No 4:40, only before 5:30pm</t>
   </si>
   <si>
     <t>222-BOOMER BOMBERS</t>
   </si>
   <si>
-    <t>NO 1/7/13-1/8/13, NO 1/12/13, NO 1/14/13-1/15/13, NO 1/27/13-1/29/13, NO 2/10/13-2/12/13, no 2/25/13-2/27/13</t>
+    <t>NO 11/7/13-11/8/13, NO 11/12/13, NO 11/14/13-11/15/13, NO 11/27/13-11/29/13, NO 12/10/13-12/12/13, no 12/25/13-12/27/13</t>
   </si>
   <si>
     <t>223-EAGLES-TURNER 2</t>
   </si>
   <si>
-    <t>Turner 6</t>
-  </si>
-  <si>
     <t>224-LEFTY'S DRILLERS</t>
   </si>
   <si>
-    <t>no 1/7/13, no 1/21/13, no 2/4/13, no 1/11/13, no 1/25/13, no 2/10/13, no 2/17/13</t>
+    <t>no 11/7/13, no 11/21/13, no 12/4/13, no 11/11/13, no 11/25/13, no 12/10/13, no 12/17/13</t>
   </si>
   <si>
     <t>Flash 3 or 4</t>
@@ -291,12 +280,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="GENERAL" numFmtId="165"/>
+    <numFmt formatCode="\$#,##0.00" numFmtId="166"/>
+    <numFmt formatCode="D\-MMM;@" numFmtId="167"/>
+    <numFmt formatCode="D\-MMM" numFmtId="168"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -305,38 +297,53 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Berlin Sans FB"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <u/>
+      <b val="true"/>
+      <u val="single"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <u/>
+      <b val="true"/>
+      <u val="single"/>
       <sz val="11"/>
       <name val="Berlin Sans FB"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <u/>
+      <b val="true"/>
+      <u val="single"/>
       <sz val="9"/>
       <name val="Berlin Sans FB"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <u/>
+      <b val="true"/>
+      <u val="single"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -356,7 +363,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Wingdings 2"/>
       <family val="1"/>
@@ -382,7 +389,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="14"/>
       <name val="Wingdings 2"/>
       <family val="1"/>
@@ -396,7 +403,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -412,207 +419,282 @@
     </fill>
   </fills>
   <borders count="3">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="165">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="66">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="55">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="166" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="12" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="13" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="13" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="166" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="168" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -620,8 +702,10 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -633,8 +717,160 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C6500"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C6500"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -646,138 +882,10 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="GENERAL" numFmtId="164"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -785,7 +893,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -844,334 +951,39 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H4" activeCellId="0" pane="topLeft" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375"/>
-    <col min="2" max="2" width="13.140625"/>
-    <col min="3" max="3" width="31.28515625"/>
-    <col min="4" max="4" width="8.7109375"/>
-    <col min="5" max="5" width="7.5703125"/>
-    <col min="6" max="6" width="7.140625"/>
-    <col min="7" max="7" width="5.85546875"/>
-    <col min="8" max="8" width="124.5703125"/>
-    <col min="9" max="9" width="20.85546875"/>
-    <col min="10" max="11" width="11.42578125"/>
-    <col min="12" max="12" width="9.7109375"/>
-    <col min="13" max="1025" width="8.7109375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.14795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.85714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.5714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.8622448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.70918367346939"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +994,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="2">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -1220,8 +1032,8 @@
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+      <c r="A3" s="17" t="n">
         <v>101</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -1234,13 +1046,15 @@
       <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="I3" s="21"/>
       <c r="J3" s="22"/>
       <c r="K3" s="23"/>
@@ -1254,33 +1068,33 @@
       <c r="S3" s="30"/>
       <c r="T3" s="30"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+      <c r="A4" s="17" t="n">
         <v>102</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4" s="33"/>
       <c r="K4" s="23"/>
-      <c r="L4" s="34"/>
+      <c r="L4" s="24"/>
       <c r="M4" s="25"/>
       <c r="N4" s="25"/>
       <c r="O4" s="26"/>
@@ -1290,174 +1104,176 @@
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+      <c r="A5" s="17" t="n">
         <v>103</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="21"/>
+        <v>18</v>
+      </c>
+      <c r="I5" s="21" t="n">
+        <v>105</v>
+      </c>
       <c r="J5" s="22"/>
       <c r="K5" s="23"/>
       <c r="L5" s="24"/>
       <c r="M5" s="20"/>
       <c r="N5" s="20"/>
-      <c r="O5" s="35"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="29"/>
       <c r="Q5" s="28"/>
       <c r="R5" s="29"/>
       <c r="S5" s="30"/>
       <c r="T5" s="30"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+      <c r="A6" s="17" t="n">
         <v>104</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I6" s="32"/>
       <c r="J6" s="33"/>
       <c r="K6" s="23"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="39"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="28"/>
       <c r="R6" s="29"/>
       <c r="S6" s="30"/>
       <c r="T6" s="30"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+      <c r="A7" s="17" t="n">
         <v>105</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="41" t="s">
+      <c r="H7" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="42"/>
+      <c r="I7" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="37"/>
       <c r="K7" s="23"/>
       <c r="L7" s="24"/>
       <c r="M7" s="20"/>
       <c r="N7" s="20"/>
-      <c r="O7" s="35"/>
+      <c r="O7" s="34"/>
       <c r="P7" s="29"/>
       <c r="Q7" s="28"/>
       <c r="R7" s="29"/>
       <c r="S7" s="30"/>
       <c r="T7" s="30"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+      <c r="A8" s="17" t="n">
         <v>106</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8" s="32"/>
       <c r="J8" s="33"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="34"/>
+      <c r="L8" s="24"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
-      <c r="O8" s="35"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="29"/>
       <c r="Q8" s="28"/>
       <c r="R8" s="29"/>
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+      <c r="A9" s="17" t="n">
         <v>107</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I9" s="32"/>
       <c r="J9" s="33"/>
@@ -1465,74 +1281,72 @@
       <c r="L9" s="24"/>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
-      <c r="O9" s="35"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="29"/>
       <c r="Q9" s="28"/>
       <c r="R9" s="29"/>
       <c r="S9" s="30"/>
       <c r="T9" s="30"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+      <c r="A10" s="17" t="n">
         <v>141</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="42"/>
+        <v>15</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="37"/>
       <c r="K10" s="23"/>
       <c r="L10" s="24"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
-      <c r="O10" s="35"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="29"/>
       <c r="Q10" s="28"/>
       <c r="R10" s="29"/>
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="11">
+      <c r="A11" s="17" t="n">
         <v>142</v>
       </c>
-      <c r="B11" s="44" t="s">
-        <v>28</v>
+      <c r="B11" s="38" t="s">
+        <v>29</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="42"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="23"/>
       <c r="L11" s="24"/>
       <c r="M11" s="25"/>
@@ -1544,12 +1358,12 @@
       <c r="S11" s="30"/>
       <c r="T11" s="30"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+      <c r="A12" s="17" t="n">
         <v>143</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>28</v>
+      <c r="B12" s="38" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>33</v>
@@ -1558,19 +1372,19 @@
       <c r="E12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="42"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="37"/>
       <c r="K12" s="23"/>
-      <c r="L12" s="45"/>
+      <c r="L12" s="39"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
       <c r="O12" s="26"/>
@@ -1580,12 +1394,12 @@
       <c r="S12" s="30"/>
       <c r="T12" s="30"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+      <c r="A13" s="17" t="n">
         <v>145</v>
       </c>
-      <c r="B13" s="44" t="s">
-        <v>28</v>
+      <c r="B13" s="38" t="s">
+        <v>29</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>35</v>
@@ -1594,19 +1408,19 @@
       <c r="E13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="43"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="33"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="34"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="24"/>
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
       <c r="O13" s="26"/>
@@ -1616,12 +1430,12 @@
       <c r="S13" s="30"/>
       <c r="T13" s="30"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+      <c r="A14" s="17" t="n">
         <v>146</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>28</v>
+      <c r="B14" s="38" t="s">
+        <v>29</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>37</v>
@@ -1630,33 +1444,33 @@
       <c r="E14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H14" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="43"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="33"/>
       <c r="K14" s="23"/>
-      <c r="L14" s="45"/>
+      <c r="L14" s="39"/>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
-      <c r="O14" s="35"/>
+      <c r="O14" s="34"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="28"/>
       <c r="R14" s="29"/>
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+      <c r="A15" s="17" t="n">
         <v>151</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="21" t="s">
@@ -1666,7 +1480,7 @@
       <c r="E15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="18" t="s">
@@ -1676,7 +1490,7 @@
         <v>42</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="42"/>
+      <c r="J15" s="37"/>
       <c r="K15" s="23"/>
       <c r="L15" s="24"/>
       <c r="M15" s="25"/>
@@ -1688,11 +1502,11 @@
       <c r="S15" s="30"/>
       <c r="T15" s="30"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+      <c r="A16" s="17" t="n">
         <v>152</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -1702,7 +1516,7 @@
       <c r="E16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G16" s="18" t="s">
@@ -1715,18 +1529,18 @@
       <c r="L16" s="24"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
-      <c r="O16" s="35"/>
+      <c r="O16" s="34"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="28"/>
       <c r="R16" s="29"/>
       <c r="S16" s="30"/>
       <c r="T16" s="30"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
+      <c r="A17" s="17" t="n">
         <v>153</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="21" t="s">
@@ -1736,7 +1550,7 @@
       <c r="E17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="18" t="s">
@@ -1746,21 +1560,21 @@
       <c r="I17" s="21"/>
       <c r="J17" s="33"/>
       <c r="K17" s="23"/>
-      <c r="L17" s="45"/>
+      <c r="L17" s="39"/>
       <c r="M17" s="20"/>
       <c r="N17" s="20"/>
-      <c r="O17" s="35"/>
+      <c r="O17" s="34"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="28"/>
       <c r="R17" s="29"/>
       <c r="S17" s="30"/>
       <c r="T17" s="30"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+      <c r="A18" s="17" t="n">
         <v>154</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="21" t="s">
@@ -1770,7 +1584,7 @@
       <c r="E18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="18" t="s">
@@ -1783,18 +1597,18 @@
       <c r="L18" s="24"/>
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
-      <c r="O18" s="35"/>
+      <c r="O18" s="34"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="28"/>
       <c r="R18" s="29"/>
       <c r="S18" s="30"/>
       <c r="T18" s="30"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+      <c r="A19" s="17" t="n">
         <v>155</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="21" t="s">
@@ -1804,31 +1618,31 @@
       <c r="E19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H19" s="21"/>
-      <c r="I19" s="43"/>
+      <c r="I19" s="32"/>
       <c r="J19" s="33"/>
       <c r="K19" s="23"/>
-      <c r="L19" s="34"/>
+      <c r="L19" s="24"/>
       <c r="M19" s="20"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="35"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="34"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="28"/>
       <c r="R19" s="29"/>
       <c r="S19" s="30"/>
       <c r="T19" s="30"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+      <c r="A20" s="17" t="n">
         <v>156</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="21" t="s">
@@ -1838,17 +1652,17 @@
       <c r="E20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="18" t="n">
         <v>1</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="42"/>
+        <v>15</v>
+      </c>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="37"/>
       <c r="K20" s="23"/>
-      <c r="L20" s="34"/>
+      <c r="L20" s="24"/>
       <c r="M20" s="25"/>
       <c r="N20" s="25"/>
       <c r="O20" s="26"/>
@@ -1858,11 +1672,11 @@
       <c r="S20" s="30"/>
       <c r="T20" s="30"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
+      <c r="A21" s="17" t="n">
         <v>208</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="21" t="s">
@@ -1872,7 +1686,7 @@
       <c r="E21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G21" s="18" t="s">
@@ -1881,10 +1695,10 @@
       <c r="H21" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="43"/>
-      <c r="J21" s="42"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="37"/>
       <c r="K21" s="23"/>
-      <c r="L21" s="34"/>
+      <c r="L21" s="24"/>
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="26"/>
@@ -1894,11 +1708,11 @@
       <c r="S21" s="30"/>
       <c r="T21" s="30"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+      <c r="A22" s="17" t="n">
         <v>207</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -1908,31 +1722,33 @@
       <c r="E22" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32" t="n">
+        <v>105</v>
+      </c>
       <c r="J22" s="33"/>
       <c r="K22" s="23"/>
-      <c r="L22" s="34"/>
+      <c r="L22" s="24"/>
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
-      <c r="O22" s="35"/>
+      <c r="O22" s="34"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="28"/>
       <c r="R22" s="29"/>
       <c r="S22" s="30"/>
       <c r="T22" s="30"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
+      <c r="A23" s="17" t="n">
         <v>2014</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="21" t="s">
@@ -1942,7 +1758,7 @@
       <c r="E23" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G23" s="18" t="s">
@@ -1951,12 +1767,12 @@
       <c r="H23" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I23" s="43">
+      <c r="I23" s="32" t="n">
         <v>222</v>
       </c>
-      <c r="J23" s="42"/>
+      <c r="J23" s="37"/>
       <c r="K23" s="23"/>
-      <c r="L23" s="34"/>
+      <c r="L23" s="24"/>
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="26"/>
@@ -1966,11 +1782,11 @@
       <c r="S23" s="30"/>
       <c r="T23" s="30"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
+      <c r="A24" s="17" t="n">
         <v>2015</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="21" t="s">
@@ -1980,31 +1796,31 @@
       <c r="E24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="21"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="42"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="37"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="34"/>
+      <c r="L24" s="24"/>
       <c r="M24" s="20"/>
       <c r="N24" s="20"/>
-      <c r="O24" s="35"/>
+      <c r="O24" s="34"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="28"/>
       <c r="R24" s="29"/>
       <c r="S24" s="30"/>
       <c r="T24" s="30"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
+      <c r="A25" s="17" t="n">
         <v>2016</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -2014,17 +1830,17 @@
       <c r="E25" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="21"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="42"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="37"/>
       <c r="K25" s="23"/>
-      <c r="L25" s="34"/>
+      <c r="L25" s="24"/>
       <c r="M25" s="25"/>
       <c r="N25" s="25"/>
       <c r="O25" s="26"/>
@@ -2034,11 +1850,11 @@
       <c r="S25" s="30"/>
       <c r="T25" s="30"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
+      <c r="A26" s="17" t="n">
         <v>2013</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="21" t="s">
@@ -2048,7 +1864,7 @@
       <c r="E26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G26" s="18" t="s">
@@ -2063,18 +1879,18 @@
       <c r="L26" s="24"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="35"/>
+      <c r="O26" s="34"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="28"/>
       <c r="R26" s="29"/>
       <c r="S26" s="30"/>
       <c r="T26" s="30"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
+      <c r="A27" s="17" t="n">
         <v>203</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="21" t="s">
@@ -2084,17 +1900,17 @@
       <c r="E27" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="42"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="37"/>
       <c r="K27" s="23"/>
-      <c r="L27" s="34"/>
+      <c r="L27" s="24"/>
       <c r="M27" s="25"/>
       <c r="N27" s="25"/>
       <c r="O27" s="26"/>
@@ -2104,11 +1920,11 @@
       <c r="S27" s="30"/>
       <c r="T27" s="30"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="48">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="28">
+      <c r="A28" s="42" t="n">
         <v>2012</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="21" t="s">
@@ -2118,7 +1934,7 @@
       <c r="E28" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G28" s="18" t="s">
@@ -2128,59 +1944,59 @@
         <v>60</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="51"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="45"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="54"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="48"/>
       <c r="R28" s="29"/>
       <c r="S28" s="30"/>
       <c r="T28" s="30"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="55">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
+      <c r="A29" s="17" t="n">
         <v>206</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="32" t="s">
         <v>62</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G29" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="43" t="s">
+      <c r="H29" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="43"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="34"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="24"/>
       <c r="M29" s="20"/>
       <c r="N29" s="20"/>
-      <c r="O29" s="35"/>
+      <c r="O29" s="34"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="28"/>
       <c r="R29" s="29"/>
       <c r="S29" s="30"/>
       <c r="T29" s="30"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="30">
+      <c r="A30" s="17" t="n">
         <v>202</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="21" t="s">
@@ -2190,15 +2006,13 @@
       <c r="E30" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="31" t="s">
-        <v>64</v>
-      </c>
+      <c r="H30" s="31"/>
       <c r="I30" s="21"/>
       <c r="J30" s="22"/>
       <c r="K30" s="23"/>
@@ -2212,105 +2026,105 @@
       <c r="S30" s="30"/>
       <c r="T30" s="30"/>
     </row>
-    <row r="31" spans="1:20" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="18" outlineLevel="0" r="31">
+      <c r="A31" s="17" t="n">
         <v>2010</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="49"/>
+      <c r="J31" s="43"/>
       <c r="K31" s="23"/>
-      <c r="L31" s="51"/>
+      <c r="L31" s="45"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="52"/>
-      <c r="P31" s="53"/>
-      <c r="Q31" s="54"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="47"/>
+      <c r="Q31" s="48"/>
       <c r="R31" s="29"/>
       <c r="S31" s="30"/>
-      <c r="T31" s="57"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="T31" s="50"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="32">
+      <c r="A32" s="17" t="n">
         <v>205</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H32" s="21"/>
-      <c r="I32" s="3">
+      <c r="I32" s="3" t="n">
         <v>225</v>
       </c>
-      <c r="J32" s="49"/>
+      <c r="J32" s="43"/>
       <c r="K32" s="23"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="59"/>
-      <c r="P32" s="60"/>
-      <c r="Q32" s="54"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="53"/>
+      <c r="Q32" s="48"/>
       <c r="R32" s="29"/>
       <c r="S32" s="30"/>
       <c r="T32" s="30"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
+      <c r="A33" s="17" t="n">
         <v>2011</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I33" s="43"/>
-      <c r="J33" s="42"/>
+        <v>68</v>
+      </c>
+      <c r="I33" s="32"/>
+      <c r="J33" s="37"/>
       <c r="K33" s="23"/>
-      <c r="L33" s="34"/>
+      <c r="L33" s="24"/>
       <c r="M33" s="25"/>
       <c r="N33" s="25"/>
       <c r="O33" s="26"/>
@@ -2320,57 +2134,57 @@
       <c r="S33" s="30"/>
       <c r="T33" s="30"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
+      <c r="A34" s="17" t="n">
         <v>209</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G34" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="I34" s="43"/>
-      <c r="J34" s="42"/>
+        <v>70</v>
+      </c>
+      <c r="I34" s="32"/>
+      <c r="J34" s="37"/>
       <c r="K34" s="23"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="62"/>
-      <c r="P34" s="63"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="27"/>
       <c r="Q34" s="28"/>
       <c r="R34" s="29"/>
       <c r="S34" s="30"/>
       <c r="T34" s="30"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
+      <c r="A35" s="17" t="n">
         <v>204</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G35" s="18" t="s">
@@ -2383,118 +2197,118 @@
       <c r="L35" s="24"/>
       <c r="M35" s="20"/>
       <c r="N35" s="20"/>
-      <c r="O35" s="35"/>
+      <c r="O35" s="34"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="28"/>
       <c r="R35" s="29"/>
       <c r="S35" s="30"/>
-      <c r="T35" s="64"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+      <c r="T35" s="54"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
+      <c r="A36" s="17" t="n">
         <v>201</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="I36" s="21" t="n">
+        <v>221</v>
       </c>
       <c r="J36" s="33"/>
       <c r="K36" s="23"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="63"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="27"/>
       <c r="Q36" s="28"/>
       <c r="R36" s="29"/>
       <c r="S36" s="30"/>
       <c r="T36" s="30"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
+      <c r="A37" s="17" t="n">
         <v>221</v>
       </c>
-      <c r="B37" s="44" t="s">
-        <v>76</v>
+      <c r="B37" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="65">
+      <c r="F37" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G37" s="65" t="s">
-        <v>19</v>
+      <c r="G37" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="I37" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="J37" s="42"/>
+        <v>76</v>
+      </c>
+      <c r="I37" s="32" t="n">
+        <v>201</v>
+      </c>
+      <c r="J37" s="37"/>
       <c r="K37" s="23"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="62"/>
-      <c r="P37" s="63"/>
-      <c r="Q37" s="39"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="28"/>
       <c r="R37" s="29"/>
       <c r="S37" s="30"/>
       <c r="T37" s="30"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
+      <c r="A38" s="17" t="n">
         <v>222</v>
       </c>
-      <c r="B38" s="44" t="s">
-        <v>76</v>
+      <c r="B38" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F38" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="I38" s="43">
+        <v>78</v>
+      </c>
+      <c r="I38" s="32" t="n">
         <v>2014</v>
       </c>
-      <c r="J38" s="42"/>
+      <c r="J38" s="37"/>
       <c r="K38" s="23"/>
-      <c r="L38" s="34"/>
+      <c r="L38" s="24"/>
       <c r="M38" s="25"/>
       <c r="N38" s="25"/>
       <c r="O38" s="26"/>
@@ -2504,71 +2318,69 @@
       <c r="S38" s="30"/>
       <c r="T38" s="30"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="39">
+      <c r="A39" s="17" t="n">
         <v>223</v>
       </c>
-      <c r="B39" s="44" t="s">
-        <v>76</v>
+      <c r="B39" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F39" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H39" s="21"/>
-      <c r="I39" s="21" t="s">
-        <v>83</v>
-      </c>
+      <c r="I39" s="21"/>
       <c r="J39" s="33"/>
       <c r="K39" s="23"/>
-      <c r="L39" s="45"/>
+      <c r="L39" s="39"/>
       <c r="M39" s="20"/>
       <c r="N39" s="20"/>
-      <c r="O39" s="35"/>
+      <c r="O39" s="34"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="28"/>
       <c r="R39" s="29"/>
       <c r="S39" s="30"/>
       <c r="T39" s="30"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="40">
+      <c r="A40" s="17" t="n">
         <v>224</v>
       </c>
-      <c r="B40" s="44" t="s">
-        <v>76</v>
+      <c r="B40" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="18">
+      <c r="F40" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="I40" s="43" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="I40" s="32" t="s">
+        <v>82</v>
       </c>
       <c r="J40" s="33"/>
       <c r="K40" s="23"/>
-      <c r="L40" s="34"/>
+      <c r="L40" s="24"/>
       <c r="M40" s="25"/>
       <c r="N40" s="25"/>
       <c r="O40" s="26"/>
@@ -2578,72 +2390,72 @@
       <c r="S40" s="30"/>
       <c r="T40" s="30"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="41">
+      <c r="A41" s="17" t="n">
         <v>225</v>
       </c>
-      <c r="B41" s="44" t="s">
-        <v>76</v>
+      <c r="B41" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="18">
+      <c r="F41" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H41" s="21"/>
-      <c r="I41" s="3">
+      <c r="I41" s="3" t="n">
         <v>205</v>
       </c>
-      <c r="J41" s="49"/>
+      <c r="J41" s="43"/>
       <c r="K41" s="23"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="60"/>
-      <c r="Q41" s="54"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="51"/>
+      <c r="O41" s="52"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="48"/>
       <c r="R41" s="29"/>
       <c r="S41" s="30"/>
       <c r="T41" s="30"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="55">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="42">
+      <c r="A42" s="17" t="n">
         <v>226</v>
       </c>
-      <c r="B42" s="44" t="s">
-        <v>76</v>
+      <c r="B42" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="18">
+      <c r="F42" s="18" t="n">
         <v>2</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="42"/>
+        <v>85</v>
+      </c>
+      <c r="I42" s="32"/>
+      <c r="J42" s="37"/>
       <c r="K42" s="23"/>
       <c r="L42" s="24"/>
       <c r="M42" s="20"/>
       <c r="N42" s="20"/>
-      <c r="O42" s="35"/>
+      <c r="O42" s="34"/>
       <c r="P42" s="29"/>
       <c r="Q42" s="28"/>
       <c r="R42" s="29"/>
@@ -2652,87 +2464,120 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" operator="duplicateValues" percent="0" priority="2" rank="0" text="" type="duplicateValues">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R9">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule aboveAverage="0" bottom="0" dxfId="1" equalAverage="0" operator="duplicateValues" percent="0" priority="3" rank="0" text="" type="duplicateValues">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R9">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
+    <cfRule aboveAverage="0" bottom="0" dxfId="2" equalAverage="0" operator="equal" percent="0" priority="4" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R9">
+    <cfRule aboveAverage="0" bottom="0" dxfId="3" equalAverage="0" operator="lessThan" percent="0" priority="5" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+    <cfRule aboveAverage="0" bottom="0" dxfId="4" equalAverage="0" operator="greaterThan" percent="0" priority="6" rank="0" text="" type="cellIs">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule aboveAverage="0" bottom="0" dxfId="5" equalAverage="0" operator="lessThan" percent="0" priority="7" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R42">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule aboveAverage="0" bottom="0" dxfId="6" equalAverage="0" operator="equal" percent="0" priority="8" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R42">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule aboveAverage="0" bottom="0" dxfId="7" equalAverage="0" operator="equal" percent="0" priority="9" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R42">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="lessThan">
+    <cfRule aboveAverage="0" bottom="0" dxfId="8" equalAverage="0" operator="lessThan" percent="0" priority="10" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="greaterThan">
+    <cfRule aboveAverage="0" bottom="0" dxfId="9" equalAverage="0" operator="greaterThan" percent="0" priority="11" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
+    <cfRule aboveAverage="0" bottom="0" dxfId="10" equalAverage="0" operator="lessThan" percent="0" priority="12" rank="0" text="" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="duplicateValues" dxfId="1" priority="14"/>
+    <cfRule aboveAverage="0" bottom="0" dxfId="11" equalAverage="0" operator="duplicateValues" percent="0" priority="13" rank="0" text="" type="duplicateValues">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
+    <cfRule aboveAverage="0" bottom="0" dxfId="12" equalAverage="0" operator="duplicateValues" percent="0" priority="14" rank="0" text="" type="duplicateValues">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
   </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
   </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>